<commit_message>
final updates, current version suppose to work
</commit_message>
<xml_diff>
--- a/grocery/grocery.xlsx
+++ b/grocery/grocery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_repo\automated_grocery_list\grocery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56237E1C-E48A-457A-B8BF-523056BD00C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1EA093-58A9-4882-AF1C-C0BA138A5262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{61C671A2-11E5-4B70-AF1E-44D95A4BDD21}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{61C671A2-11E5-4B70-AF1E-44D95A4BDD21}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="190">
   <si>
     <t>Semaine</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Sauce bbq</t>
   </si>
   <si>
-    <t>Sauce brune</t>
-  </si>
-  <si>
     <t>Sauce soya</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t>Couscous et saucisses</t>
   </si>
   <si>
-    <t>Poulet, patate pilée et sauce brune</t>
-  </si>
-  <si>
     <t>Shish taouk et patate grec</t>
   </si>
   <si>
@@ -607,6 +601,15 @@
   </si>
   <si>
     <t>Store</t>
+  </si>
+  <si>
+    <t>Appart</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>Poulet, patate pilée et sauce bbq</t>
   </si>
 </sst>
 </file>
@@ -998,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5EE295-D5EB-4158-B8A8-A538E9BFF134}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H126" sqref="H126"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,6 +1013,7 @@
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1023,7 +1027,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1036,6 +1040,9 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1047,6 +1054,9 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1058,6 +1068,9 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1069,6 +1082,9 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1080,6 +1096,9 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1091,6 +1110,9 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1102,27 +1124,36 @@
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1135,16 +1166,22 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,6 +1194,9 @@
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1168,6 +1208,9 @@
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1179,6 +1222,9 @@
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1190,8 +1236,11 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1201,8 +1250,11 @@
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1212,10 +1264,13 @@
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>14</v>
@@ -1223,8 +1278,11 @@
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1234,8 +1292,11 @@
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1245,8 +1306,11 @@
       <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1256,8 +1320,11 @@
       <c r="C22" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1267,10 +1334,13 @@
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>14</v>
@@ -1278,8 +1348,11 @@
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1289,8 +1362,11 @@
       <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1300,10 +1376,13 @@
       <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -1311,8 +1390,11 @@
       <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1322,10 +1404,13 @@
       <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>14</v>
@@ -1333,8 +1418,11 @@
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1344,10 +1432,13 @@
       <c r="C30" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>14</v>
@@ -1355,10 +1446,13 @@
       <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>14</v>
@@ -1366,10 +1460,13 @@
       <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>14</v>
@@ -1377,8 +1474,11 @@
       <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1388,8 +1488,11 @@
       <c r="C34" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1399,8 +1502,11 @@
       <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1410,8 +1516,11 @@
       <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1421,10 +1530,13 @@
       <c r="C37" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>14</v>
@@ -1432,30 +1544,39 @@
       <c r="C38" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>123</v>
-      </c>
       <c r="B40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1465,8 +1586,11 @@
       <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1476,8 +1600,11 @@
       <c r="C42" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1487,8 +1614,11 @@
       <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1498,8 +1628,11 @@
       <c r="C44" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1509,10 +1642,13 @@
       <c r="C45" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>14</v>
@@ -1520,8 +1656,11 @@
       <c r="C46" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1531,8 +1670,11 @@
       <c r="C47" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1542,8 +1684,11 @@
       <c r="C48" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1553,10 +1698,13 @@
       <c r="C49" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>14</v>
@@ -1564,8 +1712,11 @@
       <c r="C50" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1575,8 +1726,11 @@
       <c r="C51" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1586,8 +1740,11 @@
       <c r="C52" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1597,8 +1754,11 @@
       <c r="C53" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1608,8 +1768,11 @@
       <c r="C54" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1619,8 +1782,11 @@
       <c r="C55" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1630,10 +1796,13 @@
       <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>15</v>
@@ -1641,8 +1810,11 @@
       <c r="C57" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -1652,8 +1824,11 @@
       <c r="C58" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -1663,8 +1838,11 @@
       <c r="C59" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -1674,10 +1852,13 @@
       <c r="C60" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>14</v>
@@ -1685,8 +1866,11 @@
       <c r="C61" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -1696,8 +1880,11 @@
       <c r="C62" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -1707,8 +1894,11 @@
       <c r="C63" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -1718,8 +1908,11 @@
       <c r="C64" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -1729,8 +1922,11 @@
       <c r="C65" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -1740,8 +1936,11 @@
       <c r="C66" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -1751,8 +1950,11 @@
       <c r="C67" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -1762,10 +1964,13 @@
       <c r="C68" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>14</v>
@@ -1773,10 +1978,13 @@
       <c r="C69" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>15</v>
@@ -1784,8 +1992,11 @@
       <c r="C70" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -1795,8 +2006,11 @@
       <c r="C71" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -1806,10 +2020,13 @@
       <c r="C72" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>15</v>
@@ -1817,8 +2034,11 @@
       <c r="C73" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -1828,10 +2048,13 @@
       <c r="C74" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>14</v>
@@ -1839,8 +2062,11 @@
       <c r="C75" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>68</v>
       </c>
@@ -1850,8 +2076,11 @@
       <c r="C76" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>69</v>
       </c>
@@ -1861,8 +2090,11 @@
       <c r="C77" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -1872,8 +2104,11 @@
       <c r="C78" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>71</v>
       </c>
@@ -1883,8 +2118,11 @@
       <c r="C79" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>72</v>
       </c>
@@ -1894,8 +2132,11 @@
       <c r="C80" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -1905,10 +2146,13 @@
       <c r="C81" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>15</v>
@@ -1916,41 +2160,53 @@
       <c r="C82" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>126</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>133</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>127</v>
-      </c>
       <c r="B85" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -1960,8 +2216,11 @@
       <c r="C86" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -1971,8 +2230,11 @@
       <c r="C87" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -1982,8 +2244,11 @@
       <c r="C88" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -1993,8 +2258,11 @@
       <c r="C89" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>78</v>
       </c>
@@ -2004,10 +2272,13 @@
       <c r="C90" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>14</v>
@@ -2015,8 +2286,11 @@
       <c r="C91" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -2026,8 +2300,11 @@
       <c r="C92" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -2037,8 +2314,11 @@
       <c r="C93" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -2048,8 +2328,11 @@
       <c r="C94" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>82</v>
       </c>
@@ -2059,8 +2342,11 @@
       <c r="C95" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>83</v>
       </c>
@@ -2070,8 +2356,11 @@
       <c r="C96" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>84</v>
       </c>
@@ -2081,8 +2370,11 @@
       <c r="C97" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -2092,8 +2384,11 @@
       <c r="C98" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>86</v>
       </c>
@@ -2103,8 +2398,11 @@
       <c r="C99" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -2114,10 +2412,13 @@
       <c r="C100" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>14</v>
@@ -2125,8 +2426,11 @@
       <c r="C101" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -2136,10 +2440,13 @@
       <c r="C102" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>15</v>
@@ -2147,10 +2454,13 @@
       <c r="C103" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>15</v>
@@ -2158,8 +2468,11 @@
       <c r="C104" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>89</v>
       </c>
@@ -2169,8 +2482,11 @@
       <c r="C105" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>90</v>
       </c>
@@ -2180,8 +2496,11 @@
       <c r="C106" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>91</v>
       </c>
@@ -2191,8 +2510,11 @@
       <c r="C107" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>92</v>
       </c>
@@ -2202,30 +2524,39 @@
       <c r="C108" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>93</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>94</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>95</v>
       </c>
@@ -2235,30 +2566,39 @@
       <c r="C111" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>96</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>97</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>98</v>
       </c>
@@ -2268,8 +2608,11 @@
       <c r="C114" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>99</v>
       </c>
@@ -2279,8 +2622,11 @@
       <c r="C115" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>100</v>
       </c>
@@ -2288,10 +2634,13 @@
         <v>14</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>101</v>
       </c>
@@ -2299,10 +2648,13 @@
         <v>14</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>102</v>
       </c>
@@ -2312,19 +2664,25 @@
       <c r="C118" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>103</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -2334,8 +2692,11 @@
       <c r="C120" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>105</v>
       </c>
@@ -2345,8 +2706,11 @@
       <c r="C121" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>106</v>
       </c>
@@ -2356,19 +2720,25 @@
       <c r="C122" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>107</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>108</v>
       </c>
@@ -2378,30 +2748,39 @@
       <c r="C124" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>109</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>110</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>111</v>
       </c>
@@ -2411,30 +2790,39 @@
       <c r="C127" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>165</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>112</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>167</v>
-      </c>
       <c r="B129" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>113</v>
       </c>
@@ -2442,10 +2830,13 @@
         <v>14</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>114</v>
       </c>
@@ -2453,10 +2844,13 @@
         <v>14</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>115</v>
       </c>
@@ -2466,28 +2860,20 @@
       <c r="C132" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>116</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>14</v>
+      <c r="D132" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{CE5EE295-D5EB-4158-B8A8-A538E9BFF134}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D133">
-    <sortCondition ref="A2:A133"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D132">
+    <sortCondition ref="A2:A132"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B119:C1048576" xr:uid="{62FA2DBA-9F3B-4EC0-A890-91170B0463AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B118:C1048576" xr:uid="{62FA2DBA-9F3B-4EC0-A890-91170B0463AE}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:C118" xr:uid="{C9156C60-5DF4-4C3A-92F2-343AF651F593}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:C117" xr:uid="{C9156C60-5DF4-4C3A-92F2-343AF651F593}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{0AF9494F-23C4-4BE0-99A3-981AF9639D65}">
@@ -2502,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E7B79B-27E5-45CE-B6D8-0FC90E03396E}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2532,7 +2918,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2543,7 +2929,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2551,10 +2937,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2565,7 +2951,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2573,10 +2959,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2584,10 +2970,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2595,10 +2981,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2606,10 +2992,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2617,10 +3003,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2628,10 +3014,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2639,10 +3025,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2653,7 +3039,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2661,10 +3047,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2672,10 +3058,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -2683,10 +3069,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2694,10 +3080,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2708,7 +3094,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2716,10 +3102,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2727,10 +3113,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2741,7 +3127,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -2749,7 +3135,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -2760,10 +3146,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -2771,10 +3157,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -2782,10 +3168,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>